<commit_message>
Adiciona diario de bordo da turma B do CodeXP
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
+++ b/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04672685-A6FB-418E-8972-EE5815FA27A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529423D-E003-4F01-BE43-2D859F393BED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,12 +624,12 @@
 Imersão com a Linx e entrevista com o cliente</t>
   </si>
   <si>
-    <t>Aula sobre Trello.
-Utilizando Brainstorm e Design Thinking, início da construção das identidades visuais, proto-persona, ptoro-jornada e marca dos projetos e prototipação inicial, no papel, das telas do sistema</t>
+    <t>Aula sobre Adobe XD clonando a interface da home do site do mercado livre e demonstração de navegação usando o XD.
+Criação da identidade visual usando o software, além da definição do nome do projeto, paleta de cores e logotipo.</t>
   </si>
   <si>
-    <t>Aula sobre Adobe XD clonando a interface da home do site do mercado livre e demonstração de navegação usando o XD.
-Criação da identidade visual usando o software, além da definição do nome do projeto, paleta de cores e logotipo.</t>
+    <t>Aula sobre Trello.
+Utilizando Brainstorm e Design Thinking, início da construção das identidades visuais, proto-persona, proto-jornada e marca dos projetos e prototipação inicial, no papel, das telas do sistema</t>
   </si>
 </sst>
 </file>
@@ -2134,11 +2134,31 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2149,42 +2169,10 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2212,6 +2200,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3283,13 +3283,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="186" t="s">
+      <c r="A4" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="189"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -3394,9 +3394,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="188"/>
-      <c r="C5" s="177"/>
+      <c r="A5" s="179"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="179"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -3501,11 +3501,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="177"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="177"/>
+      <c r="C6" s="179"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -3610,11 +3610,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="179"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="177"/>
+      <c r="C7" s="179"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -3719,11 +3719,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="177"/>
+      <c r="A8" s="179"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="177"/>
+      <c r="C8" s="179"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -3828,11 +3828,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="177"/>
+      <c r="A9" s="179"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="177"/>
+      <c r="C9" s="179"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -3937,11 +3937,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="177"/>
+      <c r="A10" s="179"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="177"/>
+      <c r="C10" s="179"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -4046,11 +4046,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="177"/>
+      <c r="A11" s="179"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="177"/>
+      <c r="C11" s="179"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -4155,9 +4155,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="177"/>
+      <c r="A12" s="179"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="178"/>
+      <c r="C12" s="182"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -4262,10 +4262,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="190" t="s">
+      <c r="A13" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="191" t="s">
+      <c r="B13" s="184" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -4374,8 +4374,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="177"/>
-      <c r="B14" s="183"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="185"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -4496,7 +4496,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="177"/>
+      <c r="A15" s="179"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -4606,7 +4606,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="177"/>
+      <c r="A16" s="179"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -4716,7 +4716,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="177"/>
+      <c r="A17" s="179"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -4828,7 +4828,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="177"/>
+      <c r="A18" s="179"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -4938,7 +4938,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="177"/>
+      <c r="A19" s="179"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="177"/>
+      <c r="A20" s="179"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -5158,7 +5158,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="178"/>
+      <c r="A21" s="182"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="192" t="s">
+      <c r="B22" s="176" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -5379,7 +5379,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="188"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -5486,13 +5486,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="179" t="s">
+      <c r="A24" s="187" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="181">
+      <c r="C24" s="189">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -5600,11 +5600,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="180"/>
+      <c r="A25" s="188"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="177"/>
+      <c r="C25" s="179"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -5710,11 +5710,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="180"/>
+      <c r="A26" s="188"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="177"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -5820,11 +5820,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="180"/>
+      <c r="A27" s="188"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="177"/>
+      <c r="C27" s="179"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -5930,11 +5930,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="180"/>
+      <c r="A28" s="188"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="177"/>
+      <c r="C28" s="179"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -6040,11 +6040,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="180"/>
+      <c r="A29" s="188"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="177"/>
+      <c r="C29" s="179"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -6150,11 +6150,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="180"/>
+      <c r="A30" s="188"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="177"/>
+      <c r="C30" s="179"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -6260,11 +6260,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="180"/>
+      <c r="A31" s="188"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="177"/>
+      <c r="C31" s="179"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -6370,11 +6370,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="180"/>
+      <c r="A32" s="188"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="177"/>
+      <c r="C32" s="179"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -6480,11 +6480,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="180"/>
+      <c r="A33" s="188"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="177"/>
+      <c r="C33" s="179"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -6590,11 +6590,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="180"/>
+      <c r="A34" s="188"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="177"/>
+      <c r="C34" s="179"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -6700,11 +6700,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="180"/>
+      <c r="A35" s="188"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="178"/>
+      <c r="C35" s="182"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -6810,11 +6810,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="180"/>
+      <c r="A36" s="188"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="181">
+      <c r="C36" s="189">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -6922,11 +6922,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="180"/>
+      <c r="A37" s="188"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="177"/>
+      <c r="C37" s="179"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -7032,11 +7032,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="180"/>
+      <c r="A38" s="188"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="177"/>
+      <c r="C38" s="179"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -7142,11 +7142,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="180"/>
+      <c r="A39" s="188"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="177"/>
+      <c r="C39" s="179"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -7252,11 +7252,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="180"/>
+      <c r="A40" s="188"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="177"/>
+      <c r="C40" s="179"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -7362,11 +7362,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="180"/>
+      <c r="A41" s="188"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="177"/>
+      <c r="C41" s="179"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -7472,11 +7472,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="180"/>
+      <c r="A42" s="188"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="177"/>
+      <c r="C42" s="179"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -7582,11 +7582,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="180"/>
+      <c r="A43" s="188"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="177"/>
+      <c r="C43" s="179"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -7692,11 +7692,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="180"/>
+      <c r="A44" s="188"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="177"/>
+      <c r="C44" s="179"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -7802,11 +7802,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="180"/>
+      <c r="A45" s="188"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="177"/>
+      <c r="C45" s="179"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -7912,11 +7912,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="180"/>
+      <c r="A46" s="188"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="177"/>
+      <c r="C46" s="179"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8022,11 +8022,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="180"/>
+      <c r="A47" s="188"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="177"/>
+      <c r="C47" s="179"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -8140,11 +8140,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="180"/>
+      <c r="A48" s="188"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="177"/>
+      <c r="C48" s="179"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -8253,7 +8253,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="182" t="s">
+      <c r="B49" s="190" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -8363,7 +8363,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="183"/>
+      <c r="B50" s="185"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -11794,7 +11794,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="184" t="s">
+      <c r="A81" s="191" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -11906,7 +11906,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="177"/>
+      <c r="A82" s="179"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12016,7 +12016,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="177"/>
+      <c r="A83" s="179"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -12126,7 +12126,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="177"/>
+      <c r="A84" s="179"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -12236,7 +12236,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="177"/>
+      <c r="A85" s="179"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -12346,7 +12346,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="177"/>
+      <c r="A86" s="179"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -12456,7 +12456,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="177"/>
+      <c r="A87" s="179"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -12568,7 +12568,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="177"/>
+      <c r="A88" s="179"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -12678,7 +12678,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="177"/>
+      <c r="A89" s="179"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -12788,7 +12788,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="177"/>
+      <c r="A90" s="179"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -12898,11 +12898,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="177"/>
+      <c r="A91" s="179"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="185"/>
+      <c r="C91" s="192"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13008,11 +13008,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="177"/>
+      <c r="A92" s="179"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="177"/>
+      <c r="C92" s="179"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -13118,11 +13118,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="178"/>
+      <c r="A93" s="182"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="177"/>
+      <c r="C93" s="179"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -13346,7 +13346,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="176" t="s">
+      <c r="A95" s="186" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -13458,7 +13458,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="177"/>
+      <c r="A96" s="179"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -13568,7 +13568,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="177"/>
+      <c r="A97" s="179"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -13678,7 +13678,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="177"/>
+      <c r="A98" s="179"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -13788,7 +13788,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="177"/>
+      <c r="A99" s="179"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -13898,7 +13898,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="177"/>
+      <c r="A100" s="179"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14008,7 +14008,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="177"/>
+      <c r="A101" s="179"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -14118,7 +14118,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="177"/>
+      <c r="A102" s="179"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -14228,7 +14228,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="177"/>
+      <c r="A103" s="179"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -14340,7 +14340,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="177"/>
+      <c r="A104" s="179"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -14450,7 +14450,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="177"/>
+      <c r="A105" s="179"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -14568,7 +14568,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="177"/>
+      <c r="A106" s="179"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -14678,7 +14678,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="177"/>
+      <c r="A107" s="179"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -14788,7 +14788,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="177"/>
+      <c r="A108" s="179"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -14898,7 +14898,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="177"/>
+      <c r="A109" s="179"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15008,7 +15008,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="177"/>
+      <c r="A110" s="179"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -15118,7 +15118,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="177"/>
+      <c r="A111" s="179"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -15228,7 +15228,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="177"/>
+      <c r="A112" s="179"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -15338,7 +15338,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="177"/>
+      <c r="A113" s="179"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -15448,7 +15448,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="177"/>
+      <c r="A114" s="179"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -15558,7 +15558,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="177"/>
+      <c r="A115" s="179"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -15668,7 +15668,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="177"/>
+      <c r="A116" s="179"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -15794,7 +15794,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="177"/>
+      <c r="A117" s="179"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -15904,7 +15904,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="178"/>
+      <c r="A118" s="182"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -23275,12 +23275,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -23288,6 +23282,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23299,7 +23299,7 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F4" sqref="F4:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -23610,110 +23610,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="198" t="s">
+      <c r="D2" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="198" t="s">
+      <c r="E2" s="194"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="194"/>
+      <c r="K2" s="194"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="194"/>
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
+      <c r="R2" s="194" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="198"/>
-      <c r="T2" s="198"/>
-      <c r="U2" s="198"/>
-      <c r="V2" s="198"/>
-      <c r="W2" s="198"/>
-      <c r="X2" s="198"/>
-      <c r="Y2" s="198"/>
-      <c r="Z2" s="198"/>
-      <c r="AA2" s="198"/>
-      <c r="AB2" s="198"/>
-      <c r="AC2" s="198"/>
-      <c r="AD2" s="198"/>
-      <c r="AE2" s="198"/>
-      <c r="AF2" s="198"/>
-      <c r="AG2" s="198"/>
-      <c r="AH2" s="198"/>
-      <c r="AI2" s="198"/>
-      <c r="AJ2" s="198"/>
-      <c r="AK2" s="198"/>
-      <c r="AL2" s="198"/>
-      <c r="AM2" s="198" t="s">
+      <c r="S2" s="194"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="194"/>
+      <c r="V2" s="194"/>
+      <c r="W2" s="194"/>
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="194"/>
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="194"/>
+      <c r="AD2" s="194"/>
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="194"/>
+      <c r="AH2" s="194"/>
+      <c r="AI2" s="194"/>
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="194"/>
+      <c r="AL2" s="194"/>
+      <c r="AM2" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="198"/>
-      <c r="AO2" s="198"/>
-      <c r="AP2" s="198"/>
-      <c r="AQ2" s="198"/>
-      <c r="AR2" s="198"/>
-      <c r="AS2" s="198"/>
-      <c r="AT2" s="198"/>
-      <c r="AU2" s="198"/>
-      <c r="AV2" s="198"/>
-      <c r="AW2" s="198"/>
-      <c r="AX2" s="199"/>
-      <c r="AY2" s="199"/>
-      <c r="AZ2" s="199"/>
-      <c r="BA2" s="199"/>
-      <c r="BB2" s="199"/>
-      <c r="BC2" s="199"/>
-      <c r="BD2" s="199"/>
-      <c r="BE2" s="199"/>
-      <c r="BF2" s="199"/>
-      <c r="BG2" s="199"/>
-      <c r="BH2" s="199"/>
-      <c r="BI2" s="199"/>
-      <c r="BJ2" s="198" t="s">
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="194"/>
+      <c r="AP2" s="194"/>
+      <c r="AQ2" s="194"/>
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="194"/>
+      <c r="AT2" s="194"/>
+      <c r="AU2" s="194"/>
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="194"/>
+      <c r="AX2" s="195"/>
+      <c r="AY2" s="195"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="195"/>
+      <c r="BB2" s="195"/>
+      <c r="BC2" s="195"/>
+      <c r="BD2" s="195"/>
+      <c r="BE2" s="195"/>
+      <c r="BF2" s="195"/>
+      <c r="BG2" s="195"/>
+      <c r="BH2" s="195"/>
+      <c r="BI2" s="195"/>
+      <c r="BJ2" s="194" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="198"/>
-      <c r="BL2" s="198"/>
-      <c r="BM2" s="198"/>
-      <c r="BN2" s="198"/>
-      <c r="BO2" s="198"/>
-      <c r="BP2" s="198"/>
-      <c r="BQ2" s="198"/>
-      <c r="BR2" s="198"/>
-      <c r="BS2" s="198"/>
-      <c r="BT2" s="198"/>
-      <c r="BU2" s="198"/>
-      <c r="BV2" s="198"/>
-      <c r="BW2" s="198"/>
-      <c r="BX2" s="200"/>
-      <c r="BY2" s="200"/>
-      <c r="BZ2" s="200"/>
-      <c r="CA2" s="200"/>
-      <c r="CB2" s="200"/>
-      <c r="CC2" s="200"/>
-      <c r="CD2" s="200"/>
-      <c r="CE2" s="201" t="s">
+      <c r="BK2" s="194"/>
+      <c r="BL2" s="194"/>
+      <c r="BM2" s="194"/>
+      <c r="BN2" s="194"/>
+      <c r="BO2" s="194"/>
+      <c r="BP2" s="194"/>
+      <c r="BQ2" s="194"/>
+      <c r="BR2" s="194"/>
+      <c r="BS2" s="194"/>
+      <c r="BT2" s="194"/>
+      <c r="BU2" s="194"/>
+      <c r="BV2" s="194"/>
+      <c r="BW2" s="194"/>
+      <c r="BX2" s="196"/>
+      <c r="BY2" s="196"/>
+      <c r="BZ2" s="196"/>
+      <c r="CA2" s="196"/>
+      <c r="CB2" s="196"/>
+      <c r="CC2" s="196"/>
+      <c r="CD2" s="196"/>
+      <c r="CE2" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="202"/>
-      <c r="CG2" s="202"/>
-      <c r="CH2" s="202"/>
-      <c r="CI2" s="202"/>
-      <c r="CJ2" s="202"/>
-      <c r="CK2" s="202"/>
-      <c r="CL2" s="202"/>
-      <c r="CM2" s="202"/>
-      <c r="CN2" s="202"/>
-      <c r="CO2" s="202"/>
-      <c r="CP2" s="202"/>
-      <c r="CQ2" s="202"/>
-      <c r="CR2" s="202"/>
-      <c r="CS2" s="202"/>
+      <c r="CF2" s="198"/>
+      <c r="CG2" s="198"/>
+      <c r="CH2" s="198"/>
+      <c r="CI2" s="198"/>
+      <c r="CJ2" s="198"/>
+      <c r="CK2" s="198"/>
+      <c r="CL2" s="198"/>
+      <c r="CM2" s="198"/>
+      <c r="CN2" s="198"/>
+      <c r="CO2" s="198"/>
+      <c r="CP2" s="198"/>
+      <c r="CQ2" s="198"/>
+      <c r="CR2" s="198"/>
+      <c r="CS2" s="198"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -24009,24 +24009,24 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="202" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="193"/>
-      <c r="D4" s="194" t="s">
+      <c r="C4" s="203"/>
+      <c r="D4" s="204" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="203" t="s">
+      <c r="E4" s="199" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="203" t="s">
+      <c r="F4" s="199" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="199" t="s">
         <v>144</v>
-      </c>
-      <c r="G4" s="203" t="s">
-        <v>145</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -24038,22 +24038,22 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="197"/>
-      <c r="AW4" s="197"/>
-      <c r="BT4" s="197"/>
-      <c r="BW4" s="197"/>
-      <c r="CT4" s="197"/>
+      <c r="AV4" s="193"/>
+      <c r="AW4" s="193"/>
+      <c r="BT4" s="193"/>
+      <c r="BW4" s="193"/>
+      <c r="CT4" s="193"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="196"/>
-      <c r="B5" s="193" t="s">
+      <c r="A5" s="202"/>
+      <c r="B5" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="195"/>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
-      <c r="G5" s="205"/>
+      <c r="C5" s="203"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="201"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -24064,22 +24064,22 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="197"/>
-      <c r="AW5" s="197"/>
-      <c r="BT5" s="197"/>
-      <c r="BW5" s="197"/>
-      <c r="CT5" s="197"/>
+      <c r="AV5" s="193"/>
+      <c r="AW5" s="193"/>
+      <c r="BT5" s="193"/>
+      <c r="BW5" s="193"/>
+      <c r="CT5" s="193"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="196"/>
-      <c r="B6" s="193" t="s">
+      <c r="A6" s="202"/>
+      <c r="B6" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="205"/>
+      <c r="C6" s="203"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="201"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -24090,107 +24090,97 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="197"/>
-      <c r="AW6" s="197"/>
-      <c r="BT6" s="197"/>
-      <c r="BW6" s="197"/>
-      <c r="CT6" s="197"/>
+      <c r="AV6" s="193"/>
+      <c r="AW6" s="193"/>
+      <c r="BT6" s="193"/>
+      <c r="BW6" s="193"/>
+      <c r="CT6" s="193"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="196"/>
-      <c r="B7" s="193" t="s">
+      <c r="A7" s="202"/>
+      <c r="B7" s="203" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="193"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="204"/>
-      <c r="F7" s="204"/>
-      <c r="G7" s="205"/>
+      <c r="C7" s="203"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="201"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="197"/>
-      <c r="AW7" s="197"/>
-      <c r="BT7" s="197"/>
-      <c r="BW7" s="197"/>
-      <c r="CT7" s="197"/>
+      <c r="AV7" s="193"/>
+      <c r="AW7" s="193"/>
+      <c r="BT7" s="193"/>
+      <c r="BW7" s="193"/>
+      <c r="CT7" s="193"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="196" t="s">
+      <c r="A8" s="202" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="193" t="s">
+      <c r="B8" s="203" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="193"/>
-      <c r="D8" s="195"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
-      <c r="G8" s="205"/>
-      <c r="AV8" s="197"/>
-      <c r="AW8" s="197"/>
-      <c r="BT8" s="197"/>
-      <c r="BW8" s="197"/>
-      <c r="CT8" s="197"/>
+      <c r="C8" s="203"/>
+      <c r="D8" s="205"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="201"/>
+      <c r="AV8" s="193"/>
+      <c r="AW8" s="193"/>
+      <c r="BT8" s="193"/>
+      <c r="BW8" s="193"/>
+      <c r="CT8" s="193"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="196"/>
-      <c r="B9" s="193" t="s">
+      <c r="A9" s="202"/>
+      <c r="B9" s="203" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="193"/>
-      <c r="D9" s="195"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="205"/>
-      <c r="AV9" s="197"/>
-      <c r="AW9" s="197"/>
-      <c r="BT9" s="197"/>
-      <c r="BW9" s="197"/>
-      <c r="CT9" s="197"/>
+      <c r="C9" s="203"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="201"/>
+      <c r="AV9" s="193"/>
+      <c r="AW9" s="193"/>
+      <c r="BT9" s="193"/>
+      <c r="BW9" s="193"/>
+      <c r="CT9" s="193"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="196"/>
-      <c r="B10" s="193" t="s">
+      <c r="A10" s="202"/>
+      <c r="B10" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="193"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="204"/>
-      <c r="F10" s="204"/>
-      <c r="G10" s="205"/>
-      <c r="AV10" s="197"/>
-      <c r="AW10" s="197"/>
-      <c r="BT10" s="197"/>
-      <c r="BW10" s="197"/>
-      <c r="CT10" s="197"/>
+      <c r="C10" s="203"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="201"/>
+      <c r="AV10" s="193"/>
+      <c r="AW10" s="193"/>
+      <c r="BT10" s="193"/>
+      <c r="BW10" s="193"/>
+      <c r="CT10" s="193"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="196"/>
-      <c r="B11" s="193" t="s">
+      <c r="A11" s="202"/>
+      <c r="B11" s="203" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="193"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="204"/>
-      <c r="F11" s="204"/>
-      <c r="G11" s="205"/>
-      <c r="AV11" s="197"/>
-      <c r="AW11" s="197"/>
-      <c r="BT11" s="197"/>
-      <c r="BW11" s="197"/>
-      <c r="CT11" s="197"/>
+      <c r="C11" s="203"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="201"/>
+      <c r="AV11" s="193"/>
+      <c r="AW11" s="193"/>
+      <c r="BT11" s="193"/>
+      <c r="BW11" s="193"/>
+      <c r="CT11" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -24205,6 +24195,16 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D4:D11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 19-08 da turma B
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
+++ b/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529423D-E003-4F01-BE43-2D859F393BED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CodeXP-Cronograma" sheetId="3" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{8E9E8068-276E-4FC3-89A4-2DB29C38E9E7}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{CFBDF186-C884-4174-BF24-95E209780388}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{99BC0D19-82CF-42B1-BBB1-B4C6729CDB9F}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{0DD13E23-870A-43E1-BC30-7E726FEA1BF8}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{F43E15C6-9BED-4A2A-8454-C2264410B727}">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D6505B1F-B0EE-4F84-9583-541E9DDB1F76}">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{90AC5519-2E56-47B1-80E0-0BEFDA25805D}">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{240C5C0E-A999-4767-8ACD-98BDE2345359}">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="147">
   <si>
     <t>S</t>
   </si>
@@ -631,11 +630,14 @@
     <t>Aula sobre Trello.
 Utilizando Brainstorm e Design Thinking, início da construção das identidades visuais, proto-persona, proto-jornada e marca dos projetos e prototipação inicial, no papel, das telas do sistema</t>
   </si>
+  <si>
+    <t>Continuação de Identidade visual e criação de um banner para validar a a identidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23">
     <font>
       <sz val="10"/>
@@ -1793,7 +1795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2134,31 +2136,11 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2169,14 +2151,46 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2202,22 +2216,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{5785764D-B2B3-497C-84FC-10D2CF06F828}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2619,7 +2624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6A7CE2-BE31-4A6B-B6B9-3E8136F434F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3283,13 +3288,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="188" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="189" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="181"/>
+      <c r="C4" s="190"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -3394,9 +3399,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="179"/>
-      <c r="B5" s="177"/>
-      <c r="C5" s="179"/>
+      <c r="A5" s="177"/>
+      <c r="B5" s="187"/>
+      <c r="C5" s="177"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -3501,11 +3506,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="179"/>
+      <c r="A6" s="177"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="179"/>
+      <c r="C6" s="177"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -3610,11 +3615,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="179"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="179"/>
+      <c r="C7" s="177"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -3719,11 +3724,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="179"/>
+      <c r="A8" s="177"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="179"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -3828,11 +3833,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="179"/>
+      <c r="A9" s="177"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="179"/>
+      <c r="C9" s="177"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -3937,11 +3942,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="179"/>
+      <c r="A10" s="177"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="179"/>
+      <c r="C10" s="177"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -4046,11 +4051,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="179"/>
+      <c r="A11" s="177"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="179"/>
+      <c r="C11" s="177"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -4155,9 +4160,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="179"/>
+      <c r="A12" s="177"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="182"/>
+      <c r="C12" s="178"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -4262,10 +4267,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="191" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="192" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -4374,8 +4379,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="179"/>
-      <c r="B14" s="185"/>
+      <c r="A14" s="177"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -4496,7 +4501,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="179"/>
+      <c r="A15" s="177"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -4606,7 +4611,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="179"/>
+      <c r="A16" s="177"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -4716,7 +4721,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="179"/>
+      <c r="A17" s="177"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -4828,7 +4833,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="179"/>
+      <c r="A18" s="177"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -4938,7 +4943,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="179"/>
+      <c r="A19" s="177"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -5048,7 +5053,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="179"/>
+      <c r="A20" s="177"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -5158,7 +5163,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="182"/>
+      <c r="A21" s="178"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -5269,7 +5274,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="176" t="s">
+      <c r="B22" s="186" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -5379,7 +5384,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="177"/>
+      <c r="B23" s="187"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -5486,13 +5491,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="187" t="s">
+      <c r="A24" s="179" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="189">
+      <c r="C24" s="181">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -5600,11 +5605,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="188"/>
+      <c r="A25" s="180"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="179"/>
+      <c r="C25" s="177"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -5710,11 +5715,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="188"/>
+      <c r="A26" s="180"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="179"/>
+      <c r="C26" s="177"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -5820,11 +5825,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="188"/>
+      <c r="A27" s="180"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="179"/>
+      <c r="C27" s="177"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -5930,11 +5935,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="188"/>
+      <c r="A28" s="180"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="179"/>
+      <c r="C28" s="177"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -6040,11 +6045,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="188"/>
+      <c r="A29" s="180"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="179"/>
+      <c r="C29" s="177"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -6150,11 +6155,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="188"/>
+      <c r="A30" s="180"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="179"/>
+      <c r="C30" s="177"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -6260,11 +6265,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="188"/>
+      <c r="A31" s="180"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="179"/>
+      <c r="C31" s="177"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -6370,11 +6375,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="188"/>
+      <c r="A32" s="180"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="179"/>
+      <c r="C32" s="177"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -6480,11 +6485,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="188"/>
+      <c r="A33" s="180"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="179"/>
+      <c r="C33" s="177"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -6590,11 +6595,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="188"/>
+      <c r="A34" s="180"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="179"/>
+      <c r="C34" s="177"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -6700,11 +6705,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="188"/>
+      <c r="A35" s="180"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="182"/>
+      <c r="C35" s="178"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -6810,11 +6815,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="188"/>
+      <c r="A36" s="180"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="189">
+      <c r="C36" s="181">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -6922,11 +6927,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="188"/>
+      <c r="A37" s="180"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="179"/>
+      <c r="C37" s="177"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -7032,11 +7037,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="188"/>
+      <c r="A38" s="180"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="179"/>
+      <c r="C38" s="177"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -7142,11 +7147,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="188"/>
+      <c r="A39" s="180"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="179"/>
+      <c r="C39" s="177"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -7252,11 +7257,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="188"/>
+      <c r="A40" s="180"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="179"/>
+      <c r="C40" s="177"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -7362,11 +7367,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="188"/>
+      <c r="A41" s="180"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="179"/>
+      <c r="C41" s="177"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -7472,11 +7477,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="188"/>
+      <c r="A42" s="180"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="179"/>
+      <c r="C42" s="177"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -7582,11 +7587,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="188"/>
+      <c r="A43" s="180"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="179"/>
+      <c r="C43" s="177"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -7692,11 +7697,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="188"/>
+      <c r="A44" s="180"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="179"/>
+      <c r="C44" s="177"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -7802,11 +7807,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="188"/>
+      <c r="A45" s="180"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="179"/>
+      <c r="C45" s="177"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -7912,11 +7917,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="188"/>
+      <c r="A46" s="180"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="179"/>
+      <c r="C46" s="177"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8022,11 +8027,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="188"/>
+      <c r="A47" s="180"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="179"/>
+      <c r="C47" s="177"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -8140,11 +8145,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="188"/>
+      <c r="A48" s="180"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="179"/>
+      <c r="C48" s="177"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -8253,7 +8258,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="190" t="s">
+      <c r="B49" s="182" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -8363,7 +8368,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="185"/>
+      <c r="B50" s="183"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -11794,7 +11799,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="191" t="s">
+      <c r="A81" s="184" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -11906,7 +11911,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="179"/>
+      <c r="A82" s="177"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12016,7 +12021,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="179"/>
+      <c r="A83" s="177"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -12126,7 +12131,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="179"/>
+      <c r="A84" s="177"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -12236,7 +12241,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="179"/>
+      <c r="A85" s="177"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -12346,7 +12351,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="179"/>
+      <c r="A86" s="177"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -12456,7 +12461,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="179"/>
+      <c r="A87" s="177"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -12568,7 +12573,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="179"/>
+      <c r="A88" s="177"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -12678,7 +12683,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="179"/>
+      <c r="A89" s="177"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -12788,7 +12793,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="179"/>
+      <c r="A90" s="177"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -12898,11 +12903,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="179"/>
+      <c r="A91" s="177"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="192"/>
+      <c r="C91" s="185"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13008,11 +13013,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="179"/>
+      <c r="A92" s="177"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="179"/>
+      <c r="C92" s="177"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -13118,11 +13123,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="182"/>
+      <c r="A93" s="178"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="179"/>
+      <c r="C93" s="177"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -13346,7 +13351,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="186" t="s">
+      <c r="A95" s="176" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -13458,7 +13463,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="179"/>
+      <c r="A96" s="177"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -13568,7 +13573,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="179"/>
+      <c r="A97" s="177"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -13678,7 +13683,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="179"/>
+      <c r="A98" s="177"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -13788,7 +13793,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="179"/>
+      <c r="A99" s="177"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -13898,7 +13903,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="179"/>
+      <c r="A100" s="177"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14008,7 +14013,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="179"/>
+      <c r="A101" s="177"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -14118,7 +14123,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="179"/>
+      <c r="A102" s="177"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -14228,7 +14233,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="179"/>
+      <c r="A103" s="177"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -14340,7 +14345,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="179"/>
+      <c r="A104" s="177"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -14450,7 +14455,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="179"/>
+      <c r="A105" s="177"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -14568,7 +14573,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="179"/>
+      <c r="A106" s="177"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -14678,7 +14683,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="179"/>
+      <c r="A107" s="177"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -14788,7 +14793,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="179"/>
+      <c r="A108" s="177"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -14898,7 +14903,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="179"/>
+      <c r="A109" s="177"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15008,7 +15013,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="179"/>
+      <c r="A110" s="177"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -15118,7 +15123,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="179"/>
+      <c r="A111" s="177"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -15228,7 +15233,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="179"/>
+      <c r="A112" s="177"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -15338,7 +15343,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="179"/>
+      <c r="A113" s="177"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -15448,7 +15453,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="179"/>
+      <c r="A114" s="177"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -15558,7 +15563,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="179"/>
+      <c r="A115" s="177"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -15668,7 +15673,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="179"/>
+      <c r="A116" s="177"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -15794,7 +15799,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="179"/>
+      <c r="A117" s="177"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -15904,7 +15909,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="182"/>
+      <c r="A118" s="178"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -23275,6 +23280,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -23282,12 +23293,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23295,11 +23300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -23610,110 +23615,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="194" t="s">
+      <c r="D2" s="198" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="194"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="194"/>
-      <c r="K2" s="194"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="194"/>
-      <c r="N2" s="194"/>
-      <c r="O2" s="194"/>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="194"/>
-      <c r="R2" s="194" t="s">
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="194"/>
-      <c r="T2" s="194"/>
-      <c r="U2" s="194"/>
-      <c r="V2" s="194"/>
-      <c r="W2" s="194"/>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="194"/>
-      <c r="Z2" s="194"/>
-      <c r="AA2" s="194"/>
-      <c r="AB2" s="194"/>
-      <c r="AC2" s="194"/>
-      <c r="AD2" s="194"/>
-      <c r="AE2" s="194"/>
-      <c r="AF2" s="194"/>
-      <c r="AG2" s="194"/>
-      <c r="AH2" s="194"/>
-      <c r="AI2" s="194"/>
-      <c r="AJ2" s="194"/>
-      <c r="AK2" s="194"/>
-      <c r="AL2" s="194"/>
-      <c r="AM2" s="194" t="s">
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="198"/>
+      <c r="W2" s="198"/>
+      <c r="X2" s="198"/>
+      <c r="Y2" s="198"/>
+      <c r="Z2" s="198"/>
+      <c r="AA2" s="198"/>
+      <c r="AB2" s="198"/>
+      <c r="AC2" s="198"/>
+      <c r="AD2" s="198"/>
+      <c r="AE2" s="198"/>
+      <c r="AF2" s="198"/>
+      <c r="AG2" s="198"/>
+      <c r="AH2" s="198"/>
+      <c r="AI2" s="198"/>
+      <c r="AJ2" s="198"/>
+      <c r="AK2" s="198"/>
+      <c r="AL2" s="198"/>
+      <c r="AM2" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="194"/>
-      <c r="AO2" s="194"/>
-      <c r="AP2" s="194"/>
-      <c r="AQ2" s="194"/>
-      <c r="AR2" s="194"/>
-      <c r="AS2" s="194"/>
-      <c r="AT2" s="194"/>
-      <c r="AU2" s="194"/>
-      <c r="AV2" s="194"/>
-      <c r="AW2" s="194"/>
-      <c r="AX2" s="195"/>
-      <c r="AY2" s="195"/>
-      <c r="AZ2" s="195"/>
-      <c r="BA2" s="195"/>
-      <c r="BB2" s="195"/>
-      <c r="BC2" s="195"/>
-      <c r="BD2" s="195"/>
-      <c r="BE2" s="195"/>
-      <c r="BF2" s="195"/>
-      <c r="BG2" s="195"/>
-      <c r="BH2" s="195"/>
-      <c r="BI2" s="195"/>
-      <c r="BJ2" s="194" t="s">
+      <c r="AN2" s="198"/>
+      <c r="AO2" s="198"/>
+      <c r="AP2" s="198"/>
+      <c r="AQ2" s="198"/>
+      <c r="AR2" s="198"/>
+      <c r="AS2" s="198"/>
+      <c r="AT2" s="198"/>
+      <c r="AU2" s="198"/>
+      <c r="AV2" s="198"/>
+      <c r="AW2" s="198"/>
+      <c r="AX2" s="199"/>
+      <c r="AY2" s="199"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="199"/>
+      <c r="BB2" s="199"/>
+      <c r="BC2" s="199"/>
+      <c r="BD2" s="199"/>
+      <c r="BE2" s="199"/>
+      <c r="BF2" s="199"/>
+      <c r="BG2" s="199"/>
+      <c r="BH2" s="199"/>
+      <c r="BI2" s="199"/>
+      <c r="BJ2" s="198" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="194"/>
-      <c r="BL2" s="194"/>
-      <c r="BM2" s="194"/>
-      <c r="BN2" s="194"/>
-      <c r="BO2" s="194"/>
-      <c r="BP2" s="194"/>
-      <c r="BQ2" s="194"/>
-      <c r="BR2" s="194"/>
-      <c r="BS2" s="194"/>
-      <c r="BT2" s="194"/>
-      <c r="BU2" s="194"/>
-      <c r="BV2" s="194"/>
-      <c r="BW2" s="194"/>
-      <c r="BX2" s="196"/>
-      <c r="BY2" s="196"/>
-      <c r="BZ2" s="196"/>
-      <c r="CA2" s="196"/>
-      <c r="CB2" s="196"/>
-      <c r="CC2" s="196"/>
-      <c r="CD2" s="196"/>
-      <c r="CE2" s="197" t="s">
+      <c r="BK2" s="198"/>
+      <c r="BL2" s="198"/>
+      <c r="BM2" s="198"/>
+      <c r="BN2" s="198"/>
+      <c r="BO2" s="198"/>
+      <c r="BP2" s="198"/>
+      <c r="BQ2" s="198"/>
+      <c r="BR2" s="198"/>
+      <c r="BS2" s="198"/>
+      <c r="BT2" s="198"/>
+      <c r="BU2" s="198"/>
+      <c r="BV2" s="198"/>
+      <c r="BW2" s="198"/>
+      <c r="BX2" s="200"/>
+      <c r="BY2" s="200"/>
+      <c r="BZ2" s="200"/>
+      <c r="CA2" s="200"/>
+      <c r="CB2" s="200"/>
+      <c r="CC2" s="200"/>
+      <c r="CD2" s="200"/>
+      <c r="CE2" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="198"/>
-      <c r="CG2" s="198"/>
-      <c r="CH2" s="198"/>
-      <c r="CI2" s="198"/>
-      <c r="CJ2" s="198"/>
-      <c r="CK2" s="198"/>
-      <c r="CL2" s="198"/>
-      <c r="CM2" s="198"/>
-      <c r="CN2" s="198"/>
-      <c r="CO2" s="198"/>
-      <c r="CP2" s="198"/>
-      <c r="CQ2" s="198"/>
-      <c r="CR2" s="198"/>
-      <c r="CS2" s="198"/>
+      <c r="CF2" s="202"/>
+      <c r="CG2" s="202"/>
+      <c r="CH2" s="202"/>
+      <c r="CI2" s="202"/>
+      <c r="CJ2" s="202"/>
+      <c r="CK2" s="202"/>
+      <c r="CL2" s="202"/>
+      <c r="CM2" s="202"/>
+      <c r="CN2" s="202"/>
+      <c r="CO2" s="202"/>
+      <c r="CP2" s="202"/>
+      <c r="CQ2" s="202"/>
+      <c r="CR2" s="202"/>
+      <c r="CS2" s="202"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -24009,26 +24014,28 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="193" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="195" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="203"/>
-      <c r="D4" s="204" t="s">
+      <c r="C4" s="195"/>
+      <c r="D4" s="196" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="199" t="s">
+      <c r="E4" s="203" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="199" t="s">
+      <c r="F4" s="203" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="199" t="s">
+      <c r="G4" s="203" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="206" t="s">
+        <v>146</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -24038,23 +24045,23 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="193"/>
-      <c r="AW4" s="193"/>
-      <c r="BT4" s="193"/>
-      <c r="BW4" s="193"/>
-      <c r="CT4" s="193"/>
+      <c r="AV4" s="194"/>
+      <c r="AW4" s="194"/>
+      <c r="BT4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="CT4" s="194"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="202"/>
-      <c r="B5" s="203" t="s">
+      <c r="A5" s="193"/>
+      <c r="B5" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="203"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="201"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="195"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="204"/>
+      <c r="F5" s="204"/>
+      <c r="G5" s="205"/>
+      <c r="H5" s="204"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -24064,23 +24071,23 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="193"/>
-      <c r="AW5" s="193"/>
-      <c r="BT5" s="193"/>
-      <c r="BW5" s="193"/>
-      <c r="CT5" s="193"/>
+      <c r="AV5" s="194"/>
+      <c r="AW5" s="194"/>
+      <c r="BT5" s="194"/>
+      <c r="BW5" s="194"/>
+      <c r="CT5" s="194"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="202"/>
-      <c r="B6" s="203" t="s">
+      <c r="A6" s="193"/>
+      <c r="B6" s="195" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="203"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="200"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="201"/>
-      <c r="H6" s="7"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="204"/>
+      <c r="F6" s="204"/>
+      <c r="G6" s="205"/>
+      <c r="H6" s="204"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -24090,97 +24097,113 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="193"/>
-      <c r="AW6" s="193"/>
-      <c r="BT6" s="193"/>
-      <c r="BW6" s="193"/>
-      <c r="CT6" s="193"/>
+      <c r="AV6" s="194"/>
+      <c r="AW6" s="194"/>
+      <c r="BT6" s="194"/>
+      <c r="BW6" s="194"/>
+      <c r="CT6" s="194"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="202"/>
-      <c r="B7" s="203" t="s">
+      <c r="A7" s="193"/>
+      <c r="B7" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="203"/>
-      <c r="D7" s="205"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="201"/>
+      <c r="C7" s="195"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="204"/>
+      <c r="F7" s="204"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="204"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="193"/>
-      <c r="AW7" s="193"/>
-      <c r="BT7" s="193"/>
-      <c r="BW7" s="193"/>
-      <c r="CT7" s="193"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="BT7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="CT7" s="194"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="202" t="s">
+      <c r="A8" s="193" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="203" t="s">
+      <c r="B8" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="203"/>
-      <c r="D8" s="205"/>
-      <c r="E8" s="200"/>
-      <c r="F8" s="200"/>
-      <c r="G8" s="201"/>
-      <c r="AV8" s="193"/>
-      <c r="AW8" s="193"/>
-      <c r="BT8" s="193"/>
-      <c r="BW8" s="193"/>
-      <c r="CT8" s="193"/>
+      <c r="C8" s="195"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="204"/>
+      <c r="AV8" s="194"/>
+      <c r="AW8" s="194"/>
+      <c r="BT8" s="194"/>
+      <c r="BW8" s="194"/>
+      <c r="CT8" s="194"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="202"/>
-      <c r="B9" s="203" t="s">
+      <c r="A9" s="193"/>
+      <c r="B9" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="203"/>
-      <c r="D9" s="205"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="201"/>
-      <c r="AV9" s="193"/>
-      <c r="AW9" s="193"/>
-      <c r="BT9" s="193"/>
-      <c r="BW9" s="193"/>
-      <c r="CT9" s="193"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="204"/>
+      <c r="F9" s="204"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="204"/>
+      <c r="AV9" s="194"/>
+      <c r="AW9" s="194"/>
+      <c r="BT9" s="194"/>
+      <c r="BW9" s="194"/>
+      <c r="CT9" s="194"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203" t="s">
+      <c r="A10" s="193"/>
+      <c r="B10" s="195" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="203"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="201"/>
-      <c r="AV10" s="193"/>
-      <c r="AW10" s="193"/>
-      <c r="BT10" s="193"/>
-      <c r="BW10" s="193"/>
-      <c r="CT10" s="193"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="204"/>
+      <c r="F10" s="204"/>
+      <c r="G10" s="205"/>
+      <c r="H10" s="204"/>
+      <c r="AV10" s="194"/>
+      <c r="AW10" s="194"/>
+      <c r="BT10" s="194"/>
+      <c r="BW10" s="194"/>
+      <c r="CT10" s="194"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="202"/>
-      <c r="B11" s="203" t="s">
+      <c r="A11" s="193"/>
+      <c r="B11" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="203"/>
-      <c r="D11" s="205"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="201"/>
-      <c r="AV11" s="193"/>
-      <c r="AW11" s="193"/>
-      <c r="BT11" s="193"/>
-      <c r="BW11" s="193"/>
-      <c r="CT11" s="193"/>
+      <c r="C11" s="195"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="204"/>
+      <c r="G11" s="205"/>
+      <c r="H11" s="204"/>
+      <c r="AV11" s="194"/>
+      <c r="AW11" s="194"/>
+      <c r="BT11" s="194"/>
+      <c r="BW11" s="194"/>
+      <c r="CT11" s="194"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -24195,16 +24218,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D4:D11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 20-08
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
+++ b/Cronograma/CodeXp - Acompanhamento - Turma B.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
   <si>
     <t>S</t>
   </si>
@@ -632,6 +632,14 @@
   </si>
   <si>
     <t>Continuação de Identidade visual e criação de um banner para validar a a identidade</t>
+  </si>
+  <si>
+    <t>Criação do layout de baixa fidelidade de algumas páginas do projeto Gufos usando o XD.
+Início do layout de baixa fidelidade dos projetos de cada grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação do layout de alta fidelidade de algumas páginas do projeto Gufos usando o XD.
+</t>
   </si>
 </sst>
 </file>
@@ -2136,11 +2144,31 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2151,46 +2179,14 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2217,6 +2213,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3288,13 +3296,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="188" t="s">
+      <c r="A4" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="190"/>
+      <c r="C4" s="181"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -3399,9 +3407,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="187"/>
-      <c r="C5" s="177"/>
+      <c r="A5" s="179"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="179"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -3506,11 +3514,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="177"/>
+      <c r="A6" s="179"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="177"/>
+      <c r="C6" s="179"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -3615,11 +3623,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="179"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="177"/>
+      <c r="C7" s="179"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -3724,11 +3732,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="177"/>
+      <c r="A8" s="179"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="177"/>
+      <c r="C8" s="179"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -3833,11 +3841,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="177"/>
+      <c r="A9" s="179"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="177"/>
+      <c r="C9" s="179"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -3942,11 +3950,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="177"/>
+      <c r="A10" s="179"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="177"/>
+      <c r="C10" s="179"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -4051,11 +4059,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="177"/>
+      <c r="A11" s="179"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="177"/>
+      <c r="C11" s="179"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -4160,9 +4168,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="177"/>
+      <c r="A12" s="179"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="178"/>
+      <c r="C12" s="182"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -4267,10 +4275,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="191" t="s">
+      <c r="A13" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="192" t="s">
+      <c r="B13" s="184" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -4379,8 +4387,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="177"/>
-      <c r="B14" s="183"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="185"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -4501,7 +4509,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="177"/>
+      <c r="A15" s="179"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -4611,7 +4619,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="177"/>
+      <c r="A16" s="179"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -4721,7 +4729,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="177"/>
+      <c r="A17" s="179"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -4833,7 +4841,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="177"/>
+      <c r="A18" s="179"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -4943,7 +4951,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="177"/>
+      <c r="A19" s="179"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -5053,7 +5061,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="177"/>
+      <c r="A20" s="179"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -5163,7 +5171,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="178"/>
+      <c r="A21" s="182"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -5274,7 +5282,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="176" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -5384,7 +5392,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="187"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -5491,13 +5499,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="179" t="s">
+      <c r="A24" s="187" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="181">
+      <c r="C24" s="189">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -5605,11 +5613,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="180"/>
+      <c r="A25" s="188"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="177"/>
+      <c r="C25" s="179"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -5715,11 +5723,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="180"/>
+      <c r="A26" s="188"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="177"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -5825,11 +5833,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="180"/>
+      <c r="A27" s="188"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="177"/>
+      <c r="C27" s="179"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -5935,11 +5943,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="180"/>
+      <c r="A28" s="188"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="177"/>
+      <c r="C28" s="179"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -6045,11 +6053,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="180"/>
+      <c r="A29" s="188"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="177"/>
+      <c r="C29" s="179"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -6155,11 +6163,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="180"/>
+      <c r="A30" s="188"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="177"/>
+      <c r="C30" s="179"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -6265,11 +6273,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="180"/>
+      <c r="A31" s="188"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="177"/>
+      <c r="C31" s="179"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -6375,11 +6383,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="180"/>
+      <c r="A32" s="188"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="177"/>
+      <c r="C32" s="179"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -6485,11 +6493,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="180"/>
+      <c r="A33" s="188"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="177"/>
+      <c r="C33" s="179"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -6595,11 +6603,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="180"/>
+      <c r="A34" s="188"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="177"/>
+      <c r="C34" s="179"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -6705,11 +6713,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="180"/>
+      <c r="A35" s="188"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="178"/>
+      <c r="C35" s="182"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -6815,11 +6823,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="180"/>
+      <c r="A36" s="188"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="181">
+      <c r="C36" s="189">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -6927,11 +6935,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="180"/>
+      <c r="A37" s="188"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="177"/>
+      <c r="C37" s="179"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -7037,11 +7045,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="180"/>
+      <c r="A38" s="188"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="177"/>
+      <c r="C38" s="179"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -7147,11 +7155,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="180"/>
+      <c r="A39" s="188"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="177"/>
+      <c r="C39" s="179"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -7257,11 +7265,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="180"/>
+      <c r="A40" s="188"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="177"/>
+      <c r="C40" s="179"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -7367,11 +7375,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="180"/>
+      <c r="A41" s="188"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="177"/>
+      <c r="C41" s="179"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -7477,11 +7485,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="180"/>
+      <c r="A42" s="188"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="177"/>
+      <c r="C42" s="179"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -7587,11 +7595,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="180"/>
+      <c r="A43" s="188"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="177"/>
+      <c r="C43" s="179"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -7697,11 +7705,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="180"/>
+      <c r="A44" s="188"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="177"/>
+      <c r="C44" s="179"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -7807,11 +7815,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="180"/>
+      <c r="A45" s="188"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="177"/>
+      <c r="C45" s="179"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -7917,11 +7925,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="180"/>
+      <c r="A46" s="188"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="177"/>
+      <c r="C46" s="179"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8027,11 +8035,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="180"/>
+      <c r="A47" s="188"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="177"/>
+      <c r="C47" s="179"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -8145,11 +8153,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="180"/>
+      <c r="A48" s="188"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="177"/>
+      <c r="C48" s="179"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -8258,7 +8266,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="182" t="s">
+      <c r="B49" s="190" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -8368,7 +8376,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="183"/>
+      <c r="B50" s="185"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -11799,7 +11807,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="184" t="s">
+      <c r="A81" s="191" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -11911,7 +11919,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="177"/>
+      <c r="A82" s="179"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12021,7 +12029,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="177"/>
+      <c r="A83" s="179"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -12131,7 +12139,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="177"/>
+      <c r="A84" s="179"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -12241,7 +12249,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="177"/>
+      <c r="A85" s="179"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -12351,7 +12359,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="177"/>
+      <c r="A86" s="179"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -12461,7 +12469,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="177"/>
+      <c r="A87" s="179"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -12573,7 +12581,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="177"/>
+      <c r="A88" s="179"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -12683,7 +12691,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="177"/>
+      <c r="A89" s="179"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -12793,7 +12801,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="177"/>
+      <c r="A90" s="179"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -12903,11 +12911,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="177"/>
+      <c r="A91" s="179"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="185"/>
+      <c r="C91" s="192"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13013,11 +13021,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="177"/>
+      <c r="A92" s="179"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="177"/>
+      <c r="C92" s="179"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -13123,11 +13131,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="178"/>
+      <c r="A93" s="182"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="177"/>
+      <c r="C93" s="179"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -13351,7 +13359,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="176" t="s">
+      <c r="A95" s="186" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -13463,7 +13471,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="177"/>
+      <c r="A96" s="179"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -13573,7 +13581,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="177"/>
+      <c r="A97" s="179"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -13683,7 +13691,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="177"/>
+      <c r="A98" s="179"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -13793,7 +13801,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="177"/>
+      <c r="A99" s="179"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -13903,7 +13911,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="177"/>
+      <c r="A100" s="179"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14013,7 +14021,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="177"/>
+      <c r="A101" s="179"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -14123,7 +14131,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="177"/>
+      <c r="A102" s="179"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -14233,7 +14241,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="177"/>
+      <c r="A103" s="179"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -14345,7 +14353,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="177"/>
+      <c r="A104" s="179"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -14455,7 +14463,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="177"/>
+      <c r="A105" s="179"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -14573,7 +14581,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="177"/>
+      <c r="A106" s="179"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -14683,7 +14691,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="177"/>
+      <c r="A107" s="179"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -14793,7 +14801,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="177"/>
+      <c r="A108" s="179"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -14903,7 +14911,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="177"/>
+      <c r="A109" s="179"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15013,7 +15021,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="177"/>
+      <c r="A110" s="179"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -15123,7 +15131,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="177"/>
+      <c r="A111" s="179"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -15233,7 +15241,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="177"/>
+      <c r="A112" s="179"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -15343,7 +15351,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="177"/>
+      <c r="A113" s="179"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -15453,7 +15461,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="177"/>
+      <c r="A114" s="179"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -15563,7 +15571,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="177"/>
+      <c r="A115" s="179"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -15673,7 +15681,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="177"/>
+      <c r="A116" s="179"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -15799,7 +15807,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="177"/>
+      <c r="A117" s="179"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -15909,7 +15917,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="178"/>
+      <c r="A118" s="182"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -23280,12 +23288,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -23293,6 +23295,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23303,8 +23311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -23615,110 +23623,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="198" t="s">
+      <c r="D2" s="194" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="198"/>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="198" t="s">
+      <c r="E2" s="194"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="194"/>
+      <c r="K2" s="194"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="194"/>
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
+      <c r="R2" s="194" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="198"/>
-      <c r="T2" s="198"/>
-      <c r="U2" s="198"/>
-      <c r="V2" s="198"/>
-      <c r="W2" s="198"/>
-      <c r="X2" s="198"/>
-      <c r="Y2" s="198"/>
-      <c r="Z2" s="198"/>
-      <c r="AA2" s="198"/>
-      <c r="AB2" s="198"/>
-      <c r="AC2" s="198"/>
-      <c r="AD2" s="198"/>
-      <c r="AE2" s="198"/>
-      <c r="AF2" s="198"/>
-      <c r="AG2" s="198"/>
-      <c r="AH2" s="198"/>
-      <c r="AI2" s="198"/>
-      <c r="AJ2" s="198"/>
-      <c r="AK2" s="198"/>
-      <c r="AL2" s="198"/>
-      <c r="AM2" s="198" t="s">
+      <c r="S2" s="194"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="194"/>
+      <c r="V2" s="194"/>
+      <c r="W2" s="194"/>
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="194"/>
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="194"/>
+      <c r="AD2" s="194"/>
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="194"/>
+      <c r="AH2" s="194"/>
+      <c r="AI2" s="194"/>
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="194"/>
+      <c r="AL2" s="194"/>
+      <c r="AM2" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="198"/>
-      <c r="AO2" s="198"/>
-      <c r="AP2" s="198"/>
-      <c r="AQ2" s="198"/>
-      <c r="AR2" s="198"/>
-      <c r="AS2" s="198"/>
-      <c r="AT2" s="198"/>
-      <c r="AU2" s="198"/>
-      <c r="AV2" s="198"/>
-      <c r="AW2" s="198"/>
-      <c r="AX2" s="199"/>
-      <c r="AY2" s="199"/>
-      <c r="AZ2" s="199"/>
-      <c r="BA2" s="199"/>
-      <c r="BB2" s="199"/>
-      <c r="BC2" s="199"/>
-      <c r="BD2" s="199"/>
-      <c r="BE2" s="199"/>
-      <c r="BF2" s="199"/>
-      <c r="BG2" s="199"/>
-      <c r="BH2" s="199"/>
-      <c r="BI2" s="199"/>
-      <c r="BJ2" s="198" t="s">
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="194"/>
+      <c r="AP2" s="194"/>
+      <c r="AQ2" s="194"/>
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="194"/>
+      <c r="AT2" s="194"/>
+      <c r="AU2" s="194"/>
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="194"/>
+      <c r="AX2" s="195"/>
+      <c r="AY2" s="195"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="195"/>
+      <c r="BB2" s="195"/>
+      <c r="BC2" s="195"/>
+      <c r="BD2" s="195"/>
+      <c r="BE2" s="195"/>
+      <c r="BF2" s="195"/>
+      <c r="BG2" s="195"/>
+      <c r="BH2" s="195"/>
+      <c r="BI2" s="195"/>
+      <c r="BJ2" s="194" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="198"/>
-      <c r="BL2" s="198"/>
-      <c r="BM2" s="198"/>
-      <c r="BN2" s="198"/>
-      <c r="BO2" s="198"/>
-      <c r="BP2" s="198"/>
-      <c r="BQ2" s="198"/>
-      <c r="BR2" s="198"/>
-      <c r="BS2" s="198"/>
-      <c r="BT2" s="198"/>
-      <c r="BU2" s="198"/>
-      <c r="BV2" s="198"/>
-      <c r="BW2" s="198"/>
-      <c r="BX2" s="200"/>
-      <c r="BY2" s="200"/>
-      <c r="BZ2" s="200"/>
-      <c r="CA2" s="200"/>
-      <c r="CB2" s="200"/>
-      <c r="CC2" s="200"/>
-      <c r="CD2" s="200"/>
-      <c r="CE2" s="201" t="s">
+      <c r="BK2" s="194"/>
+      <c r="BL2" s="194"/>
+      <c r="BM2" s="194"/>
+      <c r="BN2" s="194"/>
+      <c r="BO2" s="194"/>
+      <c r="BP2" s="194"/>
+      <c r="BQ2" s="194"/>
+      <c r="BR2" s="194"/>
+      <c r="BS2" s="194"/>
+      <c r="BT2" s="194"/>
+      <c r="BU2" s="194"/>
+      <c r="BV2" s="194"/>
+      <c r="BW2" s="194"/>
+      <c r="BX2" s="196"/>
+      <c r="BY2" s="196"/>
+      <c r="BZ2" s="196"/>
+      <c r="CA2" s="196"/>
+      <c r="CB2" s="196"/>
+      <c r="CC2" s="196"/>
+      <c r="CD2" s="196"/>
+      <c r="CE2" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="202"/>
-      <c r="CG2" s="202"/>
-      <c r="CH2" s="202"/>
-      <c r="CI2" s="202"/>
-      <c r="CJ2" s="202"/>
-      <c r="CK2" s="202"/>
-      <c r="CL2" s="202"/>
-      <c r="CM2" s="202"/>
-      <c r="CN2" s="202"/>
-      <c r="CO2" s="202"/>
-      <c r="CP2" s="202"/>
-      <c r="CQ2" s="202"/>
-      <c r="CR2" s="202"/>
-      <c r="CS2" s="202"/>
+      <c r="CF2" s="198"/>
+      <c r="CG2" s="198"/>
+      <c r="CH2" s="198"/>
+      <c r="CI2" s="198"/>
+      <c r="CJ2" s="198"/>
+      <c r="CK2" s="198"/>
+      <c r="CL2" s="198"/>
+      <c r="CM2" s="198"/>
+      <c r="CN2" s="198"/>
+      <c r="CO2" s="198"/>
+      <c r="CP2" s="198"/>
+      <c r="CQ2" s="198"/>
+      <c r="CR2" s="198"/>
+      <c r="CS2" s="198"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -24014,30 +24022,34 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="203" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="195"/>
-      <c r="D4" s="196" t="s">
+      <c r="C4" s="204"/>
+      <c r="D4" s="205" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="203" t="s">
+      <c r="E4" s="199" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="203" t="s">
+      <c r="F4" s="199" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="203" t="s">
+      <c r="G4" s="199" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="206" t="s">
+      <c r="H4" s="202" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="202" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="202" t="s">
+        <v>148</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -24045,25 +24057,25 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
+      <c r="AV4" s="193"/>
+      <c r="AW4" s="193"/>
+      <c r="BT4" s="193"/>
+      <c r="BW4" s="193"/>
+      <c r="CT4" s="193"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="193"/>
-      <c r="B5" s="195" t="s">
+      <c r="A5" s="203"/>
+      <c r="B5" s="204" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="195"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="204"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="C5" s="204"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="201"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -24071,25 +24083,25 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
+      <c r="AV5" s="193"/>
+      <c r="AW5" s="193"/>
+      <c r="BT5" s="193"/>
+      <c r="BW5" s="193"/>
+      <c r="CT5" s="193"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="193"/>
-      <c r="B6" s="195" t="s">
+      <c r="A6" s="203"/>
+      <c r="B6" s="204" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="205"/>
-      <c r="H6" s="204"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="C6" s="204"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="201"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="200"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -24097,113 +24109,112 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
+      <c r="AV6" s="193"/>
+      <c r="AW6" s="193"/>
+      <c r="BT6" s="193"/>
+      <c r="BW6" s="193"/>
+      <c r="CT6" s="193"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="193"/>
-      <c r="B7" s="195" t="s">
+      <c r="A7" s="203"/>
+      <c r="B7" s="204" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="204"/>
-      <c r="F7" s="204"/>
-      <c r="G7" s="205"/>
-      <c r="H7" s="204"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="201"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="200"/>
+      <c r="J7" s="200"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
+      <c r="AV7" s="193"/>
+      <c r="AW7" s="193"/>
+      <c r="BT7" s="193"/>
+      <c r="BW7" s="193"/>
+      <c r="CT7" s="193"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="193" t="s">
+      <c r="A8" s="203" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="204" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="195"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="204"/>
-      <c r="F8" s="204"/>
-      <c r="G8" s="205"/>
-      <c r="H8" s="204"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="206"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="201"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="AV8" s="193"/>
+      <c r="AW8" s="193"/>
+      <c r="BT8" s="193"/>
+      <c r="BW8" s="193"/>
+      <c r="CT8" s="193"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="193"/>
-      <c r="B9" s="195" t="s">
+      <c r="A9" s="203"/>
+      <c r="B9" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="195"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="204"/>
-      <c r="G9" s="205"/>
-      <c r="H9" s="204"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
+      <c r="C9" s="204"/>
+      <c r="D9" s="206"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="AV9" s="193"/>
+      <c r="AW9" s="193"/>
+      <c r="BT9" s="193"/>
+      <c r="BW9" s="193"/>
+      <c r="CT9" s="193"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="193"/>
-      <c r="B10" s="195" t="s">
+      <c r="A10" s="203"/>
+      <c r="B10" s="204" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="195"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="204"/>
-      <c r="F10" s="204"/>
-      <c r="G10" s="205"/>
-      <c r="H10" s="204"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
+      <c r="C10" s="204"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="AV10" s="193"/>
+      <c r="AW10" s="193"/>
+      <c r="BT10" s="193"/>
+      <c r="BW10" s="193"/>
+      <c r="CT10" s="193"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="193"/>
-      <c r="B11" s="195" t="s">
+      <c r="A11" s="203"/>
+      <c r="B11" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="195"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="204"/>
-      <c r="F11" s="204"/>
-      <c r="G11" s="205"/>
-      <c r="H11" s="204"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
+      <c r="C11" s="204"/>
+      <c r="D11" s="206"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="AV11" s="193"/>
+      <c r="AW11" s="193"/>
+      <c r="BT11" s="193"/>
+      <c r="BW11" s="193"/>
+      <c r="CT11" s="193"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
+  <mergeCells count="27">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -24218,6 +24229,19 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>